<commit_message>
single spider plot added
</commit_message>
<xml_diff>
--- a/FINAL-COMBINED-DATASET.xlsx
+++ b/FINAL-COMBINED-DATASET.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="544">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="549">
   <si>
     <t xml:space="preserve">City</t>
   </si>
@@ -131,22 +131,22 @@
     <t xml:space="preserve">Population Density (per sq. km)</t>
   </si>
   <si>
-    <t xml:space="preserve">Population Change 1990 – 2000 (%)</t>
+    <t xml:space="preserve">Population Change 1990 – 2000</t>
   </si>
   <si>
-    <t xml:space="preserve">Population Change 2000 – 2010 (%)</t>
+    <t xml:space="preserve">Population Change 2000 – 2010</t>
   </si>
   <si>
-    <t xml:space="preserve">Population Change 2010 – 2020 (%)</t>
+    <t xml:space="preserve">Population Change 2010 – 2020</t>
   </si>
   <si>
-    <t xml:space="preserve">Population Change 2020 – 2025 (%)</t>
+    <t xml:space="preserve">Population Change 2020 – 2025</t>
   </si>
   <si>
     <t xml:space="preserve">Urbanization Rate 2015 (%)</t>
   </si>
   <si>
-    <t xml:space="preserve">Urbanization Rate Change 2015 – 2025 (%)</t>
+    <t xml:space="preserve">Urbanization Rate Change 2015 – 2025 (pp)</t>
   </si>
   <si>
     <t xml:space="preserve">GDP per Capita (USD)</t>
@@ -1654,6 +1654,21 @@
   <si>
     <t xml:space="preserve">MetroBike Emerging</t>
   </si>
+  <si>
+    <t xml:space="preserve">Population Change 1990 – 2000 (%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Population Change 2000 – 2010 (%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Population Change 2010 – 2020 (%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Population Change 2020 – 2025 (%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Urbanization Rate Change 2015 – 2025 (%)</t>
+  </si>
 </sst>
 </file>
 
@@ -1755,72 +1770,72 @@
   </sheetPr>
   <dimension ref="A1:BZ332"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="BN1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="CA21" activeCellId="0" sqref="CA21"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AH1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AM1" activeCellId="0" sqref="AM1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.4336734693878"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.20918367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.63775510204082"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="28.7551020408163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.63775510204082"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="21" min="18" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="5.12755102040816"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="30" min="29" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="5.80612244897959"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="40" min="37" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="4.86224489795918"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="0" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="5.80612244897959"/>
-    <col collapsed="false" hidden="false" max="51" min="51" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="52" min="52" style="0" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="53" min="53" style="0" width="6.47959183673469"/>
-    <col collapsed="false" hidden="false" max="54" min="54" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="55" min="55" style="0" width="6.20918367346939"/>
-    <col collapsed="false" hidden="false" max="56" min="56" style="0" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="57" min="57" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="58" min="58" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="59" min="59" style="0" width="5.66836734693878"/>
-    <col collapsed="false" hidden="false" max="62" min="60" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="63" min="63" style="0" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="69" min="64" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="70" min="70" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="71" min="71" style="0" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="72" min="72" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.4132653061224"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.13775510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.45918367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="28.6428571428571"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.45918367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.77551020408163"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.41326530612245"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.68367346938776"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.45918367346939"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.64285714285714"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.22448979591837"/>
+    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="11.4540816326531"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="7.50510204081633"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="7.77551020408163"/>
+    <col collapsed="false" hidden="false" max="21" min="18" style="0" width="11.4540816326531"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="7.90816326530612"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="5.05102040816327"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="11.4540816326531"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="7.90816326530612"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="11.4540816326531"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="6.54081632653061"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="7.77551020408163"/>
+    <col collapsed="false" hidden="false" max="30" min="29" style="0" width="8.3265306122449"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="6.82142857142857"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="5.73469387755102"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="6.82142857142857"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="9.13265306122449"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="6.27040816326531"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="7.50510204081633"/>
+    <col collapsed="false" hidden="false" max="40" min="37" style="0" width="9.41326530612245"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="4.78061224489796"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="8.86224489795918"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="7.77551020408163"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="9.13265306122449"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="7.22448979591837"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="6.82142857142857"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="0" width="7.37244897959184"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="0" width="7.64285714285714"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="0" width="8.5969387755102"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="5.73469387755102"/>
+    <col collapsed="false" hidden="false" max="51" min="51" style="0" width="7.37244897959184"/>
+    <col collapsed="false" hidden="false" max="52" min="52" style="0" width="6.95408163265306"/>
+    <col collapsed="false" hidden="false" max="53" min="53" style="0" width="6.41836734693878"/>
+    <col collapsed="false" hidden="false" max="54" min="54" style="0" width="7.37244897959184"/>
+    <col collapsed="false" hidden="false" max="55" min="55" style="0" width="6.13775510204082"/>
+    <col collapsed="false" hidden="false" max="56" min="56" style="0" width="7.22448979591837"/>
+    <col collapsed="false" hidden="false" max="57" min="57" style="0" width="9.81632653061224"/>
+    <col collapsed="false" hidden="false" max="58" min="58" style="0" width="11.4540816326531"/>
+    <col collapsed="false" hidden="false" max="59" min="59" style="0" width="5.58673469387755"/>
+    <col collapsed="false" hidden="false" max="62" min="60" style="0" width="11.4540816326531"/>
+    <col collapsed="false" hidden="false" max="63" min="63" style="0" width="6.95408163265306"/>
+    <col collapsed="false" hidden="false" max="69" min="64" style="0" width="11.4540816326531"/>
+    <col collapsed="false" hidden="false" max="70" min="70" style="0" width="15"/>
+    <col collapsed="false" hidden="false" max="71" min="71" style="0" width="13.780612244898"/>
+    <col collapsed="false" hidden="false" max="72" min="72" style="0" width="18.8265306122449"/>
     <col collapsed="false" hidden="false" max="73" min="73" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="74" min="74" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="74" min="74" style="0" width="12.2755102040816"/>
     <col collapsed="false" hidden="false" max="77" min="75" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="78" min="78" style="0" width="14.4438775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="79" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="78" min="78" style="0" width="14.3163265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="79" style="0" width="11.1887755102041"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -70933,11 +70948,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.780612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.1887755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.0918367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="11.1887755102041"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.6989795918367"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.1887755102041"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -71169,22 +71184,22 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E32" s="0" t="s">
-        <v>36</v>
+        <v>544</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E33" s="0" t="s">
-        <v>37</v>
+        <v>545</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E34" s="0" t="s">
-        <v>38</v>
+        <v>546</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E35" s="0" t="s">
-        <v>39</v>
+        <v>547</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -71194,7 +71209,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E37" s="0" t="s">
-        <v>41</v>
+        <v>548</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>